<commit_message>
Final commit. Program working as intended.
</commit_message>
<xml_diff>
--- a/DIDuri_Titu - Copy.xlsx
+++ b/DIDuri_Titu - Copy.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B199"/>
+  <dimension ref="A1:D252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>DID-uri DTemp</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>DID-uri DFull</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>DID-uri Comune</t>
         </is>
       </c>
@@ -449,6 +459,16 @@
           <t>$2006</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>$2006</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>$2006</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -459,6 +479,16 @@
           <t>$2047</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$2047</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$2047</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -469,6 +499,16 @@
           <t>$205F</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$205F</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$205F</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -479,6 +519,16 @@
           <t>$209B</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$209B</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$209B</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -489,6 +539,16 @@
           <t>$209D</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$209D</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$209D</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -499,6 +559,16 @@
           <t>$20CC</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$20CC</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$20CC</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -509,6 +579,16 @@
           <t>$20CD</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$20CD</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$20CD</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -519,6 +599,16 @@
           <t>$20CE</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$20CE</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$20CE</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -529,6 +619,16 @@
           <t>$20CF</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$20CF</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$20CF</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -539,6 +639,16 @@
           <t>$20D0</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$20D0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$20D0</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -549,6 +659,16 @@
           <t>$20D1</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$20D1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$20D1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -559,6 +679,16 @@
           <t>$20D3</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$20D3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$20D3</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -569,6 +699,16 @@
           <t>$2102</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$2102</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$2102</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -579,6 +719,16 @@
           <t>$2103</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$2103</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$2103</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -589,6 +739,16 @@
           <t>$2104</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$2104</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$2104</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -599,6 +759,16 @@
           <t>$2105</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$2105</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$2105</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -609,6 +779,16 @@
           <t>$2108</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$2108</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$2108</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -619,6 +799,16 @@
           <t>$210D</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$210D</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$210D</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -629,6 +819,16 @@
           <t>$210E</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$210E</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$210E</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -639,6 +839,16 @@
           <t>$210F</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$210F</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$210F</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -649,6 +859,16 @@
           <t>$2110</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>$2110</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>$2110</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -659,6 +879,16 @@
           <t>$2111</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$2111</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>$2111</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -669,6 +899,16 @@
           <t>$2112</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>$2112</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>$2112</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -679,6 +919,16 @@
           <t>$2113</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>$2113</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>$2113</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -689,6 +939,16 @@
           <t>$2114</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>$2114</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>$2114</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -699,6 +959,16 @@
           <t>$211D</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>$211D</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>$211D</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -709,6 +979,16 @@
           <t>$211E</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>$211E</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>$211E</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -719,6 +999,16 @@
           <t>$2141</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>$2141</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>$2141</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -729,6 +1019,16 @@
           <t>$2142</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>$2142</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>$2142</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -739,6 +1039,16 @@
           <t>$2143</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>$2143</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>$2143</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -749,6 +1059,16 @@
           <t>$2144</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>$2144</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>$2144</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -759,6 +1079,16 @@
           <t>$2145</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>$2145</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>$2145</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -769,6 +1099,16 @@
           <t>$2146</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>$2146</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>$2146</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -779,6 +1119,16 @@
           <t>$2147</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>$2147</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>$2147</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -789,6 +1139,16 @@
           <t>$2148</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>$2148</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>$2148</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -799,6 +1159,16 @@
           <t>$2149</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>$2149</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>$2149</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -809,6 +1179,16 @@
           <t>$214A</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>$214A</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>$214A</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -819,6 +1199,16 @@
           <t>$214B</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>$214B</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>$214B</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -829,6 +1219,16 @@
           <t>$214C</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>$214C</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>$214C</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -839,6 +1239,16 @@
           <t>$214D</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>$214D</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>$214D</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -849,6 +1259,16 @@
           <t>$214E</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>$214E</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>$214E</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -859,6 +1279,16 @@
           <t>$214F</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>$214F</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>$214F</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -869,6 +1299,16 @@
           <t>$2150</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>$2150</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>$2150</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -879,6 +1319,16 @@
           <t>$2151</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>$2151</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>$2151</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -889,6 +1339,16 @@
           <t>$2152</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>$2152</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>$2152</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -899,6 +1359,16 @@
           <t>$2153</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>$2153</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>$2153</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -909,6 +1379,16 @@
           <t>$2154</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>$2154</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>$2154</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -919,6 +1399,16 @@
           <t>$2155</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>$2155</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>$2155</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -929,6 +1419,16 @@
           <t>$2156</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>$2156</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>$2156</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -939,6 +1439,16 @@
           <t>$2157</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>$2157</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>$2157</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -949,6 +1459,16 @@
           <t>$2158</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>$2158</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>$2158</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -959,6 +1479,16 @@
           <t>$2159</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>$2159</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>$2159</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -969,6 +1499,16 @@
           <t>$215A</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>$215A</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>$215A</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -979,6 +1519,16 @@
           <t>$215B</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>$215B</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>$215B</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -989,6 +1539,16 @@
           <t>$215C</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>$215C</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>$215C</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -999,6 +1559,16 @@
           <t>$215D</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>$215D</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>$215D</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1009,6 +1579,16 @@
           <t>$2162</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>$2162</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>$2162</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1019,6 +1599,16 @@
           <t>$2165</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>$2165</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>$2165</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1029,6 +1619,16 @@
           <t>$2168</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>$2168</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>$2168</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1039,6 +1639,16 @@
           <t>$2169</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>$2169</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>$2169</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1049,6 +1659,16 @@
           <t>$216A</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>$216A</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>$216A</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1059,6 +1679,16 @@
           <t>$216B</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>$216B</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>$216B</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1069,6 +1699,16 @@
           <t>$2181</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>$2181</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>$2181</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1079,6 +1719,16 @@
           <t>$2184</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>$2184</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>$2184</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1089,6 +1739,16 @@
           <t>$219B</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>$219B</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>$219B</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1099,6 +1759,16 @@
           <t>$21A1</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>$21A1</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>$21A1</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1109,6 +1779,16 @@
           <t>$21A2</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>$21A2</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>$21A2</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1119,6 +1799,16 @@
           <t>$21A3</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>$21A3</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>$21A3</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1129,6 +1819,16 @@
           <t>$21A4</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>$21A4</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>$21A4</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1139,6 +1839,16 @@
           <t>$21A5</t>
         </is>
       </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>$21A5</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>$21A5</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1149,6 +1859,16 @@
           <t>$21A6</t>
         </is>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>$21A6</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>$21A6</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1159,6 +1879,16 @@
           <t>$21A7</t>
         </is>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>$21A7</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>$21A7</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1169,6 +1899,16 @@
           <t>$21A8</t>
         </is>
       </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>$21A8</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>$21A8</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1179,6 +1919,16 @@
           <t>$21A9</t>
         </is>
       </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>$21A9</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>$21A9</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1189,6 +1939,16 @@
           <t>$21AA</t>
         </is>
       </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>$21AA</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>$21AA</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -1199,6 +1959,16 @@
           <t>$21AB</t>
         </is>
       </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>$21AB</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>$21AB</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -1209,6 +1979,16 @@
           <t>$21AC</t>
         </is>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>$21AC</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>$21AC</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -1219,6 +1999,16 @@
           <t>$21AD</t>
         </is>
       </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>$21AD</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>$21AD</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -1229,6 +2019,16 @@
           <t>$21AE</t>
         </is>
       </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>$21AE</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>$21AE</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -1239,6 +2039,16 @@
           <t>$21AF</t>
         </is>
       </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>$21AF</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>$21AF</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -1249,6 +2059,16 @@
           <t>$21B0</t>
         </is>
       </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>$21B0</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>$21B0</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -1259,6 +2079,16 @@
           <t>$21B1</t>
         </is>
       </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>$21B1</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>$21B1</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -1269,6 +2099,16 @@
           <t>$21B2</t>
         </is>
       </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>$21B2</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>$21B2</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -1279,6 +2119,16 @@
           <t>$21B3</t>
         </is>
       </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>$21B3</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>$21B3</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -1289,6 +2139,16 @@
           <t>$21B4</t>
         </is>
       </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>$21B4</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>$21B4</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -1299,6 +2159,16 @@
           <t>$21B5</t>
         </is>
       </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>$21B5</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>$21B5</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -1309,6 +2179,16 @@
           <t>$21B6</t>
         </is>
       </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>$21B6</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>$21B6</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -1319,6 +2199,16 @@
           <t>$21B7</t>
         </is>
       </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>$21B7</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>$21B7</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -1329,6 +2219,16 @@
           <t>$21B8</t>
         </is>
       </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>$21B8</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>$21B8</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -1339,6 +2239,16 @@
           <t>$21B9</t>
         </is>
       </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>$21B9</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>$21B9</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -1349,6 +2259,16 @@
           <t>$21BA</t>
         </is>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>$21BA</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>$21BA</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -1359,6 +2279,16 @@
           <t>$21BB</t>
         </is>
       </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>$21BB</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>$21BB</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -1369,6 +2299,16 @@
           <t>$21BC</t>
         </is>
       </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>$21BC</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>$21BC</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -1379,6 +2319,16 @@
           <t>$21BD</t>
         </is>
       </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>$21BD</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>$21BD</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -1389,6 +2339,16 @@
           <t>$21BE</t>
         </is>
       </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>$21BE</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>$21BE</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -1399,6 +2359,16 @@
           <t>$21BF</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>$21BF</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>$21BF</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -1409,6 +2379,16 @@
           <t>$21C1</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>$21C1</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>$21C1</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -1419,6 +2399,16 @@
           <t>$21C2</t>
         </is>
       </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>$21C2</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>$21C2</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -1429,6 +2419,16 @@
           <t>$21C3</t>
         </is>
       </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>$21C3</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>$21C3</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -1439,6 +2439,16 @@
           <t>$21C4</t>
         </is>
       </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>$21C4</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>$21C4</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -1449,6 +2459,16 @@
           <t>$21C6</t>
         </is>
       </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>$21C6</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>$21C6</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -1459,6 +2479,16 @@
           <t>$21C7</t>
         </is>
       </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>$21C7</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>$21C7</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -1469,6 +2499,16 @@
           <t>$21C8</t>
         </is>
       </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>$21C8</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>$21C8</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -1479,6 +2519,16 @@
           <t>$222F</t>
         </is>
       </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>$222F</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>$222F</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -1489,6 +2539,16 @@
           <t>$2230</t>
         </is>
       </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>$2230</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>$2230</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -1499,6 +2559,16 @@
           <t>$223F</t>
         </is>
       </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>$223F</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>$223F</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -1509,6 +2579,16 @@
           <t>$228C</t>
         </is>
       </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>$228C</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>$228C</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -1519,6 +2599,16 @@
           <t>$228E</t>
         </is>
       </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>$228E</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>$228E</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -1529,6 +2619,16 @@
           <t>$228F</t>
         </is>
       </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>$228F</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>$228F</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -1539,6 +2639,16 @@
           <t>$2290</t>
         </is>
       </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>$2290</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>$2290</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -1549,6 +2659,16 @@
           <t>$2291</t>
         </is>
       </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>$2291</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>$2291</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -1559,6 +2679,16 @@
           <t>$2292</t>
         </is>
       </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>$2292</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>$2292</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -1569,6 +2699,16 @@
           <t>$2299</t>
         </is>
       </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>$2299</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>$2299</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -1579,6 +2719,16 @@
           <t>$22AA</t>
         </is>
       </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>$22AA</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>$22AA</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -1589,6 +2739,16 @@
           <t>$2457</t>
         </is>
       </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>$2457</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>$2457</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -1599,6 +2759,16 @@
           <t>$2458</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>$2458</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>$2458</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -1609,6 +2779,16 @@
           <t>$2459</t>
         </is>
       </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>$2459</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>$2459</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -1619,6 +2799,16 @@
           <t>$245A</t>
         </is>
       </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>$245A</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>$245A</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -1629,6 +2819,16 @@
           <t>$245B</t>
         </is>
       </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>$245B</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>$245B</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -1639,6 +2839,16 @@
           <t>$245C</t>
         </is>
       </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>$245C</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>$245C</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -1649,6 +2859,16 @@
           <t>$245D</t>
         </is>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>$245D</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>$245D</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -1659,6 +2879,16 @@
           <t>$247A</t>
         </is>
       </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>$247A</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>$247A</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -1666,6 +2896,16 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
+          <t>$24A8</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>$24C9</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
           <t>$24C9</t>
         </is>
       </c>
@@ -1676,6 +2916,16 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
+          <t>$24C9</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>$24DD</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
           <t>$24DD</t>
         </is>
       </c>
@@ -1686,6 +2936,16 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
+          <t>$24DD</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>$2501</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
           <t>$2501</t>
         </is>
       </c>
@@ -1696,6 +2956,16 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
+          <t>$2501</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>$2502</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
           <t>$2502</t>
         </is>
       </c>
@@ -1706,6 +2976,16 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
+          <t>$2502</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>$2503</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
           <t>$2503</t>
         </is>
       </c>
@@ -1716,6 +2996,16 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
+          <t>$2503</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>$2504</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
           <t>$2504</t>
         </is>
       </c>
@@ -1726,6 +3016,16 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
+          <t>$2504</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>$2505</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
           <t>$2505</t>
         </is>
       </c>
@@ -1736,6 +3036,16 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
+          <t>$2505</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>$2536</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
           <t>$2536</t>
         </is>
       </c>
@@ -1746,6 +3056,16 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
+          <t>$2536</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>$2847</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
           <t>$2847</t>
         </is>
       </c>
@@ -1756,6 +3076,16 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
+          <t>$2847</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>$2848</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
           <t>$2848</t>
         </is>
       </c>
@@ -1766,6 +3096,16 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
+          <t>$2848</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>$2849</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
           <t>$2849</t>
         </is>
       </c>
@@ -1776,6 +3116,16 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
+          <t>$2849</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>$284A</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
           <t>$284A</t>
         </is>
       </c>
@@ -1786,6 +3136,16 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
+          <t>$284A</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>$2851</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
           <t>$2851</t>
         </is>
       </c>
@@ -1796,6 +3156,16 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
+          <t>$2851</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>$2852</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
           <t>$2852</t>
         </is>
       </c>
@@ -1806,6 +3176,16 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
+          <t>$2852</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>$285F</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
           <t>$285F</t>
         </is>
       </c>
@@ -1816,6 +3196,16 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
+          <t>$285F</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>$2865</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
           <t>$2865</t>
         </is>
       </c>
@@ -1826,6 +3216,16 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
+          <t>$2865</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>$2866</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
           <t>$2866</t>
         </is>
       </c>
@@ -1836,6 +3236,16 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
+          <t>$2866</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>$2867</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
           <t>$2867</t>
         </is>
       </c>
@@ -1846,6 +3256,16 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
+          <t>$2867</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>$288D</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
           <t>$288D</t>
         </is>
       </c>
@@ -1856,6 +3276,16 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
+          <t>$288D</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>$288E</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
           <t>$288E</t>
         </is>
       </c>
@@ -1866,6 +3296,16 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
+          <t>$288E</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>$291D</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
           <t>$291D</t>
         </is>
       </c>
@@ -1876,6 +3316,16 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
+          <t>$291D</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>$291E</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
           <t>$291E</t>
         </is>
       </c>
@@ -1886,6 +3336,16 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
+          <t>$291E</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>$29DF</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
           <t>$29DF</t>
         </is>
       </c>
@@ -1896,6 +3356,16 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
+          <t>$29DF</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>$29E1</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
           <t>$29E1</t>
         </is>
       </c>
@@ -1906,6 +3376,16 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
+          <t>$29E1</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>$2A31</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
           <t>$2A31</t>
         </is>
       </c>
@@ -1916,6 +3396,16 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
+          <t>$2A31</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>$2A44</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
           <t>$2A44</t>
         </is>
       </c>
@@ -1926,6 +3416,16 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
+          <t>$2A44</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>$2A45</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
           <t>$2A45</t>
         </is>
       </c>
@@ -1936,6 +3436,16 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
+          <t>$2A45</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>$2A46</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
           <t>$2A46</t>
         </is>
       </c>
@@ -1946,6 +3456,16 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
+          <t>$2A46</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>$2AF9</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
           <t>$2AF9</t>
         </is>
       </c>
@@ -1956,6 +3476,16 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
+          <t>$2AF9</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>$2B34</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
           <t>$2B34</t>
         </is>
       </c>
@@ -1966,6 +3496,16 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
+          <t>$2B34</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>$2B59</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
           <t>$2B59</t>
         </is>
       </c>
@@ -1976,6 +3516,16 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
+          <t>$2B59</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>$2B63</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
           <t>$2B63</t>
         </is>
       </c>
@@ -1986,6 +3536,16 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
+          <t>$2B63</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>$3114</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
           <t>$3114</t>
         </is>
       </c>
@@ -1996,6 +3556,16 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
+          <t>$2BF7</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>$2897</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
           <t>$2897</t>
         </is>
       </c>
@@ -2006,6 +3576,16 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
+          <t>$30BE</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>$2B4F</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
           <t>$2B4F</t>
         </is>
       </c>
@@ -2016,6 +3596,16 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
+          <t>$30F8</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>$2BDE</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
           <t>$2BDE</t>
         </is>
       </c>
@@ -2026,6 +3616,16 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
+          <t>$3105</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>$206E</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
           <t>$206E</t>
         </is>
       </c>
@@ -2036,6 +3636,16 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
+          <t>$3106</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>$209A</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
           <t>$216D</t>
         </is>
       </c>
@@ -2046,6 +3656,16 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
+          <t>$3107</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>$216D</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
           <t>$247B</t>
         </is>
       </c>
@@ -2056,6 +3676,16 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
+          <t>$3108</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>$247B</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
           <t>$24C3</t>
         </is>
       </c>
@@ -2066,6 +3696,16 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
+          <t>$3109</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>$24C3</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
           <t>$2862</t>
         </is>
       </c>
@@ -2076,6 +3716,16 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
+          <t>$310F</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>$2862</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
           <t>$29C3</t>
         </is>
       </c>
@@ -2086,6 +3736,16 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
+          <t>$3114</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>$29C3</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
           <t>$29C4</t>
         </is>
       </c>
@@ -2096,6 +3756,16 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
+          <t>$313B</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>$29C4</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
           <t>$29C5</t>
         </is>
       </c>
@@ -2106,6 +3776,16 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
+          <t>$3149</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>$29C5</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
           <t>$29C6</t>
         </is>
       </c>
@@ -2116,6 +3796,16 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
+          <t>$314B</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>$29C6</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
           <t>$29C7</t>
         </is>
       </c>
@@ -2126,6 +3816,16 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
+          <t>$3154</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>$29C7</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
           <t>$29C8</t>
         </is>
       </c>
@@ -2136,6 +3836,16 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
+          <t>$3155</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>$29C8</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
           <t>$29C9</t>
         </is>
       </c>
@@ -2146,6 +3856,16 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
+          <t>$3169</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>$29C9</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
           <t>$29CA</t>
         </is>
       </c>
@@ -2156,6 +3876,16 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
+          <t>$316A</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>$29CA</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
           <t>$29CB</t>
         </is>
       </c>
@@ -2166,6 +3896,16 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
+          <t>$316F</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>$29CB</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
           <t>$29CC</t>
         </is>
       </c>
@@ -2176,6 +3916,16 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
+          <t>$3170</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>$29CC</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
           <t>$29CD</t>
         </is>
       </c>
@@ -2186,6 +3936,16 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
+          <t>$3171</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>$29CD</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
           <t>$29CE</t>
         </is>
       </c>
@@ -2196,6 +3956,16 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
+          <t>$3172</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>$29CE</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
           <t>$29CF</t>
         </is>
       </c>
@@ -2206,6 +3976,16 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
+          <t>$3173</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>$29CF</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
           <t>$29D0</t>
         </is>
       </c>
@@ -2216,6 +3996,16 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
+          <t>$3174</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>$29D0</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
           <t>$29D1</t>
         </is>
       </c>
@@ -2226,6 +4016,16 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
+          <t>$3175</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>$29D1</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
           <t>$29D2</t>
         </is>
       </c>
@@ -2236,6 +4036,16 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
+          <t>$3176</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>$29D2</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
           <t>$29D3</t>
         </is>
       </c>
@@ -2246,6 +4056,16 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
+          <t>$317A</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>$29D3</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
           <t>$29D4</t>
         </is>
       </c>
@@ -2256,6 +4076,16 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
+          <t>$2897</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>$29D4</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
           <t>$29D5</t>
         </is>
       </c>
@@ -2266,6 +4096,16 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
+          <t>$2B4F</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>$29D5</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
           <t>$29D6</t>
         </is>
       </c>
@@ -2276,6 +4116,16 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
+          <t>$2BDE</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>$29D6</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
           <t>$29D7</t>
         </is>
       </c>
@@ -2286,6 +4136,16 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
+          <t>$313A</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>$29D7</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
           <t>$29D8</t>
         </is>
       </c>
@@ -2296,6 +4156,16 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
+          <t>$3243</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>$29D8</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
           <t>$29D9</t>
         </is>
       </c>
@@ -2306,6 +4176,16 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
+          <t>$3244</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>$29D9</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
           <t>$29DA</t>
         </is>
       </c>
@@ -2316,6 +4196,16 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
+          <t>$3263</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>$29DA</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
           <t>$29DB</t>
         </is>
       </c>
@@ -2326,6 +4216,16 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
+          <t>$206E</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>$29DB</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
           <t>$29DC</t>
         </is>
       </c>
@@ -2336,6 +4236,16 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
+          <t>$216D</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>$29DC</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
           <t>$29DD</t>
         </is>
       </c>
@@ -2346,6 +4256,16 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
+          <t>$247B</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>$29DD</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
           <t>$29DE</t>
         </is>
       </c>
@@ -2356,6 +4276,16 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
+          <t>$24C3</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>$29DE</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
           <t>$2A26</t>
         </is>
       </c>
@@ -2366,6 +4296,16 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
+          <t>$2862</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>$2A26</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
           <t>$2A27</t>
         </is>
       </c>
@@ -2376,6 +4316,16 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
+          <t>$29C3</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>$2A27</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
           <t>$2A28</t>
         </is>
       </c>
@@ -2386,6 +4336,16 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
+          <t>$29C4</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>$2A28</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
           <t>$2AB6</t>
         </is>
       </c>
@@ -2396,6 +4356,16 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
+          <t>$29C5</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>$2AB6</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
           <t>$2AFC</t>
         </is>
       </c>
@@ -2406,6 +4376,16 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
+          <t>$29C6</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>$2AFC</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
           <t>$2AFD</t>
         </is>
       </c>
@@ -2416,9 +4396,663 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
+          <t>$29C7</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>$2AFD</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
           <t>$F1A2</t>
         </is>
       </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>$29C8</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>$2B36</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr"/>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>$29C9</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>$F1A2</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr"/>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>$29CA</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr"/>
+      <c r="D202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>$29CB</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr"/>
+      <c r="D203" t="inlineStr"/>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>$29CC</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr"/>
+      <c r="D204" t="inlineStr"/>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>$29CD</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr"/>
+      <c r="D205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>$29CE</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>$29CF</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr"/>
+      <c r="D207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>$29D0</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr"/>
+      <c r="D208" t="inlineStr"/>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>$29D1</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>$29D2</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr"/>
+      <c r="D210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>$29D3</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr"/>
+      <c r="D211" t="inlineStr"/>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>$29D4</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr"/>
+      <c r="D212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>$29D5</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr"/>
+      <c r="D213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>$29D6</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr"/>
+      <c r="D214" t="inlineStr"/>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>$29D7</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr"/>
+      <c r="D215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>$29D8</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr"/>
+      <c r="D216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>$29D9</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr"/>
+      <c r="D217" t="inlineStr"/>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>$29DA</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr"/>
+      <c r="D218" t="inlineStr"/>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>$29DB</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr"/>
+      <c r="D219" t="inlineStr"/>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>$29DC</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr"/>
+      <c r="D220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>$29DD</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr"/>
+      <c r="D221" t="inlineStr"/>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>$29DE</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr"/>
+      <c r="D222" t="inlineStr"/>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>$2A26</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr"/>
+      <c r="D223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>$2A27</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr"/>
+      <c r="D224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>$2A28</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr"/>
+      <c r="D225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>$2AB6</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr"/>
+      <c r="D226" t="inlineStr"/>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>$2AFC</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr"/>
+      <c r="D227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>$2AFD</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr"/>
+      <c r="D228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>$30D6</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr"/>
+      <c r="D229" t="inlineStr"/>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>$30D7</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr"/>
+      <c r="D230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>$30D8</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr"/>
+      <c r="D231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>230</v>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>$30D9</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr"/>
+      <c r="D232" t="inlineStr"/>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>231</v>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>$30DA</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr"/>
+      <c r="D233" t="inlineStr"/>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>232</v>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>$30DB</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr"/>
+      <c r="D234" t="inlineStr"/>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>233</v>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>$30DC</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr"/>
+      <c r="D235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>$30DD</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr"/>
+      <c r="D236" t="inlineStr"/>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>235</v>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>$30DE</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr"/>
+      <c r="D237" t="inlineStr"/>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>236</v>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>$30DF</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr"/>
+      <c r="D238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>237</v>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>$30E1</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr"/>
+      <c r="D239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>$30E2</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr"/>
+      <c r="D240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>$30E3</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr"/>
+      <c r="D241" t="inlineStr"/>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>240</v>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>$30E5</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr"/>
+      <c r="D242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>241</v>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>$30E6</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr"/>
+      <c r="D243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>242</v>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>$30E7</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr"/>
+      <c r="D244" t="inlineStr"/>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>243</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>$30E8</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr"/>
+      <c r="D245" t="inlineStr"/>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>244</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>$30F6</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr"/>
+      <c r="D246" t="inlineStr"/>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>$3193</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr"/>
+      <c r="D247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>246</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>$3194</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr"/>
+      <c r="D248" t="inlineStr"/>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>247</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>$31A8</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr"/>
+      <c r="D249" t="inlineStr"/>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>$3283</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr"/>
+      <c r="D250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>249</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>$32CB</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr"/>
+      <c r="D251" t="inlineStr"/>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>250</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>$F1A2</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr"/>
+      <c r="D252" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>